<commit_message>
replaced data with training set only
</commit_message>
<xml_diff>
--- a/Data_dictionary_ProstateCancer.xlsx
+++ b/Data_dictionary_ProstateCancer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/belalelsiesy/Downloads/RE__Filling_in_website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/belalelsiesy/Documents/UTSW STARS/Prostate Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E67DB19-068B-BE42-928A-1B30A0304897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38D2048-450F-9040-9BAD-9C2AA2125128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CoreTable" sheetId="7" r:id="rId1"/>
@@ -2773,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5756,7 +5756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>

</xml_diff>